<commit_message>
well2PLC file updated, 2022 well realignment corrections added
</commit_message>
<xml_diff>
--- a/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
+++ b/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://interainc-my.sharepoint.com/personal/rweatherl_intera_com/Documents/Documents/GitHub/100HR3-Rebound/data/pumping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EAF7FCC-BA1B-4475-A939-4875DF838A2A}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1C6F355-BDE4-4390-897C-A614CC95D022}"/>
   <bookViews>
-    <workbookView xWindow="-285" yWindow="525" windowWidth="35640" windowHeight="19725" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
+    <workbookView xWindow="165" yWindow="270" windowWidth="44940" windowHeight="19815" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="530">
   <si>
     <t>PLC_ID</t>
   </si>
@@ -1633,13 +1633,19 @@
   </si>
   <si>
     <t>199-D5-160</t>
+  </si>
+  <si>
+    <t>Disconnected in Jun 2016. Converted to 199-D4-39 INJECTION in June 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Converted to 199-D4-39 INJECTION (MJ02) in June 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1651,6 +1657,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1694,7 +1707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1715,6 +1728,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2032,8 +2046,8 @@
   <dimension ref="A1:AA154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T157" sqref="T157"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X68" sqref="X68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6615,12 +6629,11 @@
       <c r="O73" t="s">
         <v>273</v>
       </c>
-      <c r="P73" t="str">
-        <f t="shared" si="4"/>
-        <v>199-D4-39</v>
-      </c>
-      <c r="R73" t="s">
-        <v>273</v>
+      <c r="P73" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="R73" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="S73" t="s">
         <v>272</v>
@@ -6636,7 +6649,10 @@
       </c>
       <c r="W73">
         <f t="shared" ref="W73:W136" si="5">IF(R73=V73,0,1)</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="X73" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -9844,8 +9860,8 @@
       <c r="P123" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="R123" t="s">
-        <v>87</v>
+      <c r="R123" s="8" t="s">
+        <v>527</v>
       </c>
       <c r="S123" t="s">
         <v>431</v>
@@ -9874,8 +9890,8 @@
       <c r="P124" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="R124" t="s">
-        <v>87</v>
+      <c r="R124" s="8" t="s">
+        <v>525</v>
       </c>
       <c r="S124" t="s">
         <v>433</v>
@@ -9980,12 +9996,11 @@
       <c r="O126" t="s">
         <v>87</v>
       </c>
-      <c r="P126" t="str">
-        <f t="shared" si="4"/>
-        <v>spare</v>
-      </c>
-      <c r="R126" t="s">
-        <v>87</v>
+      <c r="P126" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="R126" s="10" t="s">
+        <v>273</v>
       </c>
       <c r="S126" t="s">
         <v>439</v>
@@ -10001,7 +10016,7 @@
         <v>1</v>
       </c>
       <c r="X126" s="2" t="s">
-        <v>438</v>
+        <v>528</v>
       </c>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
edited pumping data, wellinfo/wellrates, created mnw2_rr2 with updated Qrates
</commit_message>
<xml_diff>
--- a/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
+++ b/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://interainc-my.sharepoint.com/personal/rweatherl_intera_com/Documents/Documents/GitHub/100HR3-Rebound/data/pumping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1C6F355-BDE4-4390-897C-A614CC95D022}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39C52175-2B1E-43FB-A0E2-8664BD41C40D}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="270" windowWidth="44940" windowHeight="19815" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
+    <workbookView xWindow="21690" yWindow="675" windowWidth="28515" windowHeight="19155" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1635,10 +1635,23 @@
     <t>199-D5-160</t>
   </si>
   <si>
-    <t>Disconnected in Jun 2016. Converted to 199-D4-39 INJECTION in June 2023</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Converted to 199-D4-39 INJECTION (MJ02) in June 2023</t>
+  </si>
+  <si>
+    <r>
+      <t>Disconnected in Jun 2016. Converted to 199-D4-39 INJECTION in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> June 2023</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2046,8 +2059,8 @@
   <dimension ref="A1:AA154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X68" sqref="X68"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" activeCellId="1" sqref="A123:XFD123 A124:XFD124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6652,7 +6665,7 @@
         <v>1</v>
       </c>
       <c r="X73" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -9877,7 +9890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>433</v>
       </c>
@@ -10016,7 +10029,7 @@
         <v>1</v>
       </c>
       <c r="X126" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
debugged mnw2 package to oct 2023
</commit_message>
<xml_diff>
--- a/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
+++ b/data/pumping/P&T_Well_to_PLC-ID_HXDX_072023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://interainc-my.sharepoint.com/personal/rweatherl_intera_com/Documents/Documents/GitHub/100HR3-Rebound/data/pumping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39C52175-2B1E-43FB-A0E2-8664BD41C40D}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{E332A041-2BFC-42E6-99D3-287D3055A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52F34BE4-C942-4BE7-8581-2892D29A622C}"/>
   <bookViews>
-    <workbookView xWindow="21690" yWindow="675" windowWidth="28515" windowHeight="19155" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
+    <workbookView xWindow="-120" yWindow="2655" windowWidth="24330" windowHeight="15345" xr2:uid="{FAE7A2E0-1086-4996-B504-00BEF4B3D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2058,9 +2058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B50094-54B1-4969-87F6-063D779A44F3}">
   <dimension ref="A1:AA154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A124" activeCellId="1" sqref="A123:XFD123 A124:XFD124"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2287,7 @@
         <v>24</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
+        <f>IF(R3=V3,0,1)</f>
         <v>1</v>
       </c>
       <c r="X3" s="2" t="s">

</xml_diff>